<commit_message>
Documentation working, structured as R package
</commit_message>
<xml_diff>
--- a/output/pert_map_w_ids.xlsx
+++ b/output/pert_map_w_ids.xlsx
@@ -435,7 +435,7 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Construct ID</t>
+          <t>construct</t>
         </is>
       </c>
     </row>
@@ -509,7 +509,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Ctcf_1</t>
+          <t>Ctcf_CDS_1</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Rnf2_1</t>
+          <t>Rnf2_CDS_1</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Ehmt2_1</t>
+          <t>Ehmt2_CDS_1</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Parp1_1</t>
+          <t>Parp1_CDS_1</t>
         </is>
       </c>
     </row>
@@ -805,7 +805,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Parp1_2</t>
+          <t>Parp1_CDS_2</t>
         </is>
       </c>
     </row>
@@ -879,7 +879,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Zfp57_1</t>
+          <t>Zfp57_CDS_1</t>
         </is>
       </c>
     </row>
@@ -953,7 +953,7 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Atf7ip_1</t>
+          <t>Atf7ip_CDS_1</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Hdac2_1</t>
+          <t>Hdac2_CDS_1</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Kmt5a_1</t>
+          <t>Kmt5a_CDS_1</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Suv39h1_1</t>
+          <t>Suv39h1_CDS_1</t>
         </is>
       </c>
     </row>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Smchd1_1</t>
+          <t>Smchd1_CDS_1</t>
         </is>
       </c>
     </row>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Sirt1_1</t>
+          <t>Sirt1_CDS_1</t>
         </is>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Atrx_1</t>
+          <t>Atrx_CDS_1</t>
         </is>
       </c>
     </row>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Rad21_1</t>
+          <t>Rad21_CDS_1</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Eed_1</t>
+          <t>Eed_3UTR_1</t>
         </is>
       </c>
     </row>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Hdac1_1</t>
+          <t>Hdac1_CDS_1</t>
         </is>
       </c>
     </row>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Dnmt1_1</t>
+          <t>Dnmt1_CDS_1</t>
         </is>
       </c>
     </row>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Eed_2</t>
+          <t>Eed_CDS_2</t>
         </is>
       </c>
     </row>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Rrm2_1</t>
+          <t>Rrm2_CDS_1</t>
         </is>
       </c>
     </row>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Atrx_2</t>
+          <t>Atrx_CDS_2</t>
         </is>
       </c>
     </row>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Dnmt1_2</t>
+          <t>Dnmt1_CDS_2</t>
         </is>
       </c>
     </row>
@@ -2063,7 +2063,7 @@
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Sirt1_2</t>
+          <t>Sirt1_CDS_2</t>
         </is>
       </c>
     </row>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Parp1_3</t>
+          <t>Parp1_3UTR_3</t>
         </is>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Hdac2_2</t>
+          <t>Hdac2_CDS_2</t>
         </is>
       </c>
     </row>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Smchd1_2</t>
+          <t>Smchd1_CDS_2</t>
         </is>
       </c>
     </row>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Ehmt2_2</t>
+          <t>Ehmt2_CDS_2</t>
         </is>
       </c>
     </row>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Rrm2_2</t>
+          <t>Rrm2_CDS_2</t>
         </is>
       </c>
     </row>
@@ -2507,7 +2507,7 @@
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Rrm2_3</t>
+          <t>Rrm2_CDS_3</t>
         </is>
       </c>
     </row>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Smchd1_3</t>
+          <t>Smchd1_CDS_3</t>
         </is>
       </c>
     </row>
@@ -2655,7 +2655,7 @@
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Rrm2_4</t>
+          <t>Rrm2_CDS_4</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Kmt5a_2</t>
+          <t>Kmt5a_CDS_2</t>
         </is>
       </c>
     </row>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>LUCIFERASE_1</t>
+          <t>LUCIFERASE_CDS</t>
         </is>
       </c>
     </row>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Dnmt1_3</t>
+          <t>Dnmt1_CDS_3</t>
         </is>
       </c>
     </row>
@@ -2945,7 +2945,7 @@
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Dnmt1_4</t>
+          <t>Dnmt1_3UTR_4</t>
         </is>
       </c>
     </row>
@@ -3019,7 +3019,7 @@
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Rad21_2</t>
+          <t>Rad21_CDS_2</t>
         </is>
       </c>
     </row>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Ring1_1</t>
+          <t>Ring1_CDS_1</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Ehmt2_3</t>
+          <t>Ehmt2_3UTR_3</t>
         </is>
       </c>
     </row>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Rrm2_5</t>
+          <t>Rrm2_CDS_5</t>
         </is>
       </c>
     </row>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Ring1_2</t>
+          <t>Ring1_CDS_2</t>
         </is>
       </c>
     </row>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Kmt5a_3</t>
+          <t>Kmt5a_CDS_3</t>
         </is>
       </c>
     </row>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Ehmt2_4</t>
+          <t>Ehmt2_CDS_4</t>
         </is>
       </c>
     </row>
@@ -3537,7 +3537,7 @@
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Ctcf_2</t>
+          <t>Ctcf_CDS_2</t>
         </is>
       </c>
     </row>
@@ -3611,7 +3611,7 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Suv39h1_2</t>
+          <t>Suv39h1_CDS_2</t>
         </is>
       </c>
     </row>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Atrx_3</t>
+          <t>Atrx_CDS_3</t>
         </is>
       </c>
     </row>
@@ -3753,7 +3753,7 @@
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>GFP_1</t>
+          <t>GFP_CDS</t>
         </is>
       </c>
     </row>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Hdac2_3</t>
+          <t>Hdac2_CDS_3</t>
         </is>
       </c>
     </row>
@@ -3895,7 +3895,7 @@
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Hdac2_4</t>
+          <t>Hdac2_CDS_4</t>
         </is>
       </c>
     </row>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Smchd1_4</t>
+          <t>Smchd1_CDS_4</t>
         </is>
       </c>
     </row>
@@ -4043,7 +4043,7 @@
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Eed_3</t>
+          <t>Eed_CDS_3</t>
         </is>
       </c>
     </row>
@@ -4117,7 +4117,7 @@
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Atf7ip_2</t>
+          <t>Atf7ip_CDS_2</t>
         </is>
       </c>
     </row>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Eed_4</t>
+          <t>Eed_CDS_4</t>
         </is>
       </c>
     </row>
@@ -4265,7 +4265,7 @@
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Rad21_3</t>
+          <t>Rad21_3UTR_3</t>
         </is>
       </c>
     </row>
@@ -4339,7 +4339,7 @@
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Hdac1_2</t>
+          <t>Hdac1_3UTR_2</t>
         </is>
       </c>
     </row>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Rad21_4</t>
+          <t>Rad21_CDS_4</t>
         </is>
       </c>
     </row>
@@ -4487,7 +4487,7 @@
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Ehmt2_5</t>
+          <t>Ehmt2_CDS_5</t>
         </is>
       </c>
     </row>
@@ -4561,7 +4561,7 @@
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Rnf2_2</t>
+          <t>Rnf2_CDS_2</t>
         </is>
       </c>
     </row>
@@ -4635,7 +4635,7 @@
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Kmt5a_4</t>
+          <t>Kmt5a_CDS_4</t>
         </is>
       </c>
     </row>
@@ -4709,7 +4709,7 @@
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Sirt1_3</t>
+          <t>Sirt1_CDS_3</t>
         </is>
       </c>
     </row>
@@ -4783,7 +4783,7 @@
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Zfp57_2</t>
+          <t>Zfp57_CDS_2</t>
         </is>
       </c>
     </row>
@@ -4857,7 +4857,7 @@
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Ring1_3</t>
+          <t>Ring1_CDS_3</t>
         </is>
       </c>
     </row>
@@ -4931,7 +4931,7 @@
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Hdac1_3</t>
+          <t>Hdac1_CDS_3</t>
         </is>
       </c>
     </row>
@@ -5005,7 +5005,7 @@
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Sirt1_4</t>
+          <t>Sirt1_CDS_4</t>
         </is>
       </c>
     </row>
@@ -5079,7 +5079,7 @@
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Atf7ip_3</t>
+          <t>Atf7ip_CDS_3</t>
         </is>
       </c>
     </row>
@@ -5153,7 +5153,7 @@
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Parp1_4</t>
+          <t>Parp1_CDS_4</t>
         </is>
       </c>
     </row>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Dnmt1_5</t>
+          <t>Dnmt1_CDS_5</t>
         </is>
       </c>
     </row>
@@ -5301,7 +5301,7 @@
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Ctcf_3</t>
+          <t>Ctcf_CDS_3</t>
         </is>
       </c>
     </row>
@@ -5375,7 +5375,7 @@
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Zfp57_3</t>
+          <t>Zfp57_CDS_3</t>
         </is>
       </c>
     </row>
@@ -5449,7 +5449,7 @@
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Ctcf_4</t>
+          <t>Ctcf_CDS_4</t>
         </is>
       </c>
     </row>
@@ -5523,7 +5523,7 @@
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Rad21_5</t>
+          <t>Rad21_CDS_5</t>
         </is>
       </c>
     </row>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Rnf2_3</t>
+          <t>Rnf2_3UTR_3</t>
         </is>
       </c>
     </row>
@@ -5671,7 +5671,7 @@
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Hdac1_4</t>
+          <t>Hdac1_CDS_4</t>
         </is>
       </c>
     </row>
@@ -5745,7 +5745,7 @@
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Suv39h1_3</t>
+          <t>Suv39h1_3UTR_3</t>
         </is>
       </c>
     </row>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Suv39h1_4</t>
+          <t>Suv39h1_CDS_4</t>
         </is>
       </c>
     </row>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Zfp57_4</t>
+          <t>Zfp57_CDS_4</t>
         </is>
       </c>
     </row>
@@ -5967,7 +5967,7 @@
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Smchd1_5</t>
+          <t>Smchd1_3UTR_5</t>
         </is>
       </c>
     </row>
@@ -6041,7 +6041,7 @@
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Atf7ip_4</t>
+          <t>Atf7ip_CDS_4</t>
         </is>
       </c>
     </row>
@@ -6109,7 +6109,7 @@
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Ring1_4</t>
+          <t>Ring1_CDS_4</t>
         </is>
       </c>
     </row>
@@ -6183,7 +6183,7 @@
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Atf7ip_5</t>
+          <t>Atf7ip_CDS_5</t>
         </is>
       </c>
     </row>
@@ -6257,7 +6257,7 @@
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Eed_5</t>
+          <t>Eed_CDS_5</t>
         </is>
       </c>
     </row>
@@ -6331,7 +6331,7 @@
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Ctcf_5</t>
+          <t>Ctcf_CDS_5</t>
         </is>
       </c>
     </row>
@@ -6405,7 +6405,7 @@
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Sirt1_5</t>
+          <t>Sirt1_CDS_5</t>
         </is>
       </c>
     </row>
@@ -6479,7 +6479,7 @@
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Zfp57_5</t>
+          <t>Zfp57_CDS_5</t>
         </is>
       </c>
     </row>
@@ -6553,7 +6553,7 @@
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Hdac2_5</t>
+          <t>Hdac2_CDS_5</t>
         </is>
       </c>
     </row>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="P85" t="inlineStr">
         <is>
-          <t>Kmt5a_5</t>
+          <t>Kmt5a_3UTR_5</t>
         </is>
       </c>
     </row>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>Ring1_5</t>
+          <t>Ring1_CDS_5</t>
         </is>
       </c>
     </row>
@@ -6775,7 +6775,7 @@
       </c>
       <c r="P87" t="inlineStr">
         <is>
-          <t>Atrx_4</t>
+          <t>Atrx_CDS_4</t>
         </is>
       </c>
     </row>
@@ -6849,7 +6849,7 @@
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Parp1_5</t>
+          <t>Parp1_CDS_5</t>
         </is>
       </c>
     </row>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="P89" t="inlineStr">
         <is>
-          <t>Rnf2_4</t>
+          <t>Rnf2_CDS_4</t>
         </is>
       </c>
     </row>
@@ -6997,7 +6997,7 @@
       </c>
       <c r="P90" t="inlineStr">
         <is>
-          <t>Atrx_5</t>
+          <t>Atrx_CDS_5</t>
         </is>
       </c>
     </row>
@@ -7071,7 +7071,7 @@
       </c>
       <c r="P91" t="inlineStr">
         <is>
-          <t>Suv39h1_5</t>
+          <t>Suv39h1_CDS_5</t>
         </is>
       </c>
     </row>
@@ -7145,7 +7145,7 @@
       </c>
       <c r="P92" t="inlineStr">
         <is>
-          <t>Hdac1_5</t>
+          <t>Hdac1_3UTR_5</t>
         </is>
       </c>
     </row>
@@ -7219,7 +7219,7 @@
       </c>
       <c r="P93" t="inlineStr">
         <is>
-          <t>Rnf2_5</t>
+          <t>Rnf2_CDS_5</t>
         </is>
       </c>
     </row>
@@ -7287,7 +7287,7 @@
       </c>
       <c r="P94" t="inlineStr">
         <is>
-          <t>NA_</t>
+          <t>NA_NA_1</t>
         </is>
       </c>
     </row>
@@ -7355,7 +7355,7 @@
       </c>
       <c r="P95" t="inlineStr">
         <is>
-          <t>NA_</t>
+          <t>NA_NA_2</t>
         </is>
       </c>
     </row>
@@ -7423,7 +7423,7 @@
       </c>
       <c r="P96" t="inlineStr">
         <is>
-          <t>NA_</t>
+          <t>NA_NA_3</t>
         </is>
       </c>
     </row>
@@ -7491,7 +7491,7 @@
       </c>
       <c r="P97" t="inlineStr">
         <is>
-          <t>NA_</t>
+          <t>NA_NA_4</t>
         </is>
       </c>
     </row>

</xml_diff>